<commit_message>
update of vensim model
</commit_message>
<xml_diff>
--- a/data/EV sales evolution.xlsx
+++ b/data/EV sales evolution.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s203679_dtu_dk/Documents/Dokumenter/DTU_Man/h2_system_dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{223B7C6A-7B8E-4202-8BC5-0712743516B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8BCF039-0C77-4100-81F1-648914508A02}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DBD8A8F-F316-443C-87D1-727D0819F185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{B07AFFA4-5168-49DD-A7D1-B697F5C484A2}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{B07AFFA4-5168-49DD-A7D1-B697F5C484A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Global EV stocks" sheetId="1" r:id="rId1"/>
     <sheet name="EV sales share" sheetId="2" r:id="rId2"/>
+    <sheet name="Market penetration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -92,12 +94,18 @@
   <si>
     <t>Japan</t>
   </si>
+  <si>
+    <t>https://www.euronews.com/green/2023/05/08/norway-germany-uk-which-european-countries-have-the-biggest-share-of-electric-cars</t>
+  </si>
+  <si>
+    <t>For Europe:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +123,14 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,12 +157,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,6 +586,477 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global EV stocks'!$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Global EV stocks'!$K$23:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3DDC-4CFC-A0A0-356AB7BFEA6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="294382224"/>
+        <c:axId val="294383664"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Global EV stocks'!$J$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Year</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Global EV stocks'!$I$24:$I$32</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>2014</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2015</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2017</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2021</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2022</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-3DDC-4CFC-A0A0-356AB7BFEA6B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="294382224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="294383664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="294383664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="294382224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2125,6 +2613,492 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Market penetration'!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.44042432195975501"/>
+                  <c:y val="0.51231226305045208"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Market penetration'!$J$5:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Market penetration'!$K$5:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-D4D2-40A4-8657-B75057BB5425}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Market penetration'!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.1852979002624672"/>
+                  <c:y val="3.1183289588801399E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Market penetration'!$J$9:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Market penetration'!$K$9:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D4D2-40A4-8657-B75057BB5425}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="476202448"/>
+        <c:axId val="476202928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="476202448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="476202928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="476202928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="476202448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2205,6 +3179,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2722,6 +3736,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3321,15 +4851,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>515017</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>505492</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>73407</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3353,14 +4883,94 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3238500"/>
-          <a:ext cx="4782217" cy="2734057"/>
+          <a:off x="12792075" y="0"/>
+          <a:ext cx="4782217" cy="2740407"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>349798</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>718</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B0A687E-47AA-3D0D-1597-A36CC553A8FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3219450"/>
+          <a:ext cx="4616998" cy="3829768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{953E0F73-AA06-B712-AF22-7032AA2B3F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3414,16 +5024,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>396875</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>415925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3431,6 +5041,91 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A9386C1-8013-9BCF-F33B-FA80F014D6DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>79032</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2588E355-DD73-FFE0-FFB4-67E2C0FF4B1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4886325" cy="4270032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37AE52E8-D1CF-6B98-9A77-0FF9AAA65277}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3768,10 +5463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CDA5FB-724A-4250-B386-CF2FA7CD1382}">
-  <dimension ref="I1:M16"/>
+  <dimension ref="I1:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4064,8 +5759,231 @@
         <v>0.4759306170020457</v>
       </c>
     </row>
+    <row r="19" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I20" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>2013</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>0.05</v>
+      </c>
+      <c r="L23">
+        <f>K23-0</f>
+        <v>0.05</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>2014</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="L24:L32" si="2">K24-K23</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" ref="M24:M32" si="3">L24/K23</f>
+        <v>0.40000000000000008</v>
+      </c>
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>2015</v>
+      </c>
+      <c r="J25">
+        <v>6</v>
+      </c>
+      <c r="K25">
+        <v>0.12</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="3"/>
+        <v>0.71428571428571408</v>
+      </c>
+    </row>
+    <row r="26" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>2016</v>
+      </c>
+      <c r="J26">
+        <v>7</v>
+      </c>
+      <c r="K26">
+        <v>0.2</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666685</v>
+      </c>
+    </row>
+    <row r="27" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>2017</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>0.3</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999989</v>
+      </c>
+    </row>
+    <row r="28" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>2018</v>
+      </c>
+      <c r="J28">
+        <v>9</v>
+      </c>
+      <c r="K28">
+        <v>0.4</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>0.10000000000000003</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333348</v>
+      </c>
+    </row>
+    <row r="29" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>2019</v>
+      </c>
+      <c r="J29">
+        <v>10</v>
+      </c>
+      <c r="K29">
+        <v>0.6</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999989</v>
+      </c>
+    </row>
+    <row r="30" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>2020</v>
+      </c>
+      <c r="J30">
+        <v>11</v>
+      </c>
+      <c r="K30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333359</v>
+      </c>
+    </row>
+    <row r="31" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>2021</v>
+      </c>
+      <c r="J31">
+        <v>12</v>
+      </c>
+      <c r="K31">
+        <v>1.9</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="3"/>
+        <v>0.72727272727272707</v>
+      </c>
+    </row>
+    <row r="32" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>2022</v>
+      </c>
+      <c r="J32">
+        <v>13</v>
+      </c>
+      <c r="K32">
+        <v>3.1</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="3"/>
+        <v>0.63157894736842113</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" s="2">
+        <f>AVERAGE(M23:M32)</f>
+        <v>0.53064707222601959</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4074,8 +5992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AE4937-8D92-4B58-AE67-76DAC29A5FE3}">
   <dimension ref="I1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M17" sqref="J11:M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4370,7 +6288,237 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FBFFE58-EB44-4B4E-BCF7-54AA9D9E0621}">
+  <dimension ref="I1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>2013</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <f>K5-0</f>
+        <v>2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>2014</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L13" si="0">K6-K5</f>
+        <v>2</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" ref="M6:M13" si="1">L6/K5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>2015</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>2016</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>2017</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>2018</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>2019</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>24</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>2020</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>44</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="13" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2021</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>76</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="14" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="2">
+        <f>AVERAGE(M5:M14)</f>
+        <v>0.52710437710437708</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e8132505-76f9-4137-ae7c-79276eeb74ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010031884995E9A9A64AA3A22F4FAF40DDA5" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="ca4027ca244ec95ac2a7293896e2fce0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e8132505-76f9-4137-ae7c-79276eeb74ea" xmlns:ns4="7578888b-be12-48a9-baea-4639ac51bf0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e166ac659dc9ea60bab1c63573ae38b8" ns3:_="" ns4:_="">
     <xsd:import namespace="e8132505-76f9-4137-ae7c-79276eeb74ea"/>
@@ -4591,7 +6739,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4600,15 +6748,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e8132505-76f9-4137-ae7c-79276eeb74ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D838360-3748-4AD1-8E37-0EADD9368F64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e8132505-76f9-4137-ae7c-79276eeb74ea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7578888b-be12-48a9-baea-4639ac51bf0c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{107EC6BD-6D31-4D24-8D57-E2D9B40000AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4627,27 +6784,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812B9AE7-7F0E-4195-8BA0-CC6F91C78908}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D838360-3748-4AD1-8E37-0EADD9368F64}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e8132505-76f9-4137-ae7c-79276eeb74ea"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7578888b-be12-48a9-baea-4639ac51bf0c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>